<commit_message>
Fixes #32 isReverse - no longer depends on sheet order
</commit_message>
<xml_diff>
--- a/test_data/reverse.xlsx
+++ b/test_data/reverse.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pt/working/language-research-technology/ro-crate-excel/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D595512-DDED-3744-93B1-695689A4EE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94CA6F8-9337-AF48-BEF5-2A5D8AEF7AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17980" yWindow="-26960" windowWidth="35360" windowHeight="18440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17980" yWindow="-26960" windowWidth="42900" windowHeight="22640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RepositoryObject" sheetId="1" r:id="rId1"/>
-    <sheet name="File" sheetId="2" r:id="rId2"/>
+    <sheet name="File" sheetId="2" r:id="rId1"/>
+    <sheet name="RepositoryObject" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -493,77 +493,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="271" zoomScaleNormal="271" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="271" zoomScaleNormal="271" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -794,4 +731,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>